<commit_message>
Work in progress: Advanced pipeline implementation
</commit_message>
<xml_diff>
--- a/notebooks/output_complete/model_report.xlsx
+++ b/notebooks/output_complete/model_report.xlsx
@@ -457,11 +457,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RandomForest</t>
+          <t>XGBoost</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8511475547090035</v>
+        <v>0.8568094525436677</v>
       </c>
     </row>
   </sheetData>
@@ -546,35 +546,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(-0.001, 0.0449]</t>
+          <t>(-0.001, 0.0102]</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10.025</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>11.8</v>
+        <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F2" t="n">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G2" t="n">
-        <v>1.774999999999999</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="H2" t="n">
-        <v>0.002893561659452003</v>
+        <v>0.000953101798043247</v>
       </c>
       <c r="I2" t="n">
-        <v>0.02417268736678944</v>
+        <v>0.005410111043602228</v>
       </c>
       <c r="J2" t="n">
-        <v>0.02384636372471669</v>
+        <v>0.005115886218845844</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002893561659452003</v>
+        <v>0.000953101798043247</v>
       </c>
     </row>
     <row r="3">
@@ -583,35 +583,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(0.0449, 0.0848]</t>
+          <t>(0.0102, 0.0239]</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9.975000000000001</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>7.1</v>
+        <v>9.700000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="F3" t="n">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="G3" t="n">
-        <v>-2.875000000000001</v>
+        <v>-0.3000000000000003</v>
       </c>
       <c r="H3" t="n">
-        <v>0.009774631388448911</v>
+        <v>9.13776224541258e-05</v>
       </c>
       <c r="I3" t="n">
-        <v>0.06636495399496825</v>
+        <v>0.01648161187767982</v>
       </c>
       <c r="J3" t="n">
-        <v>0.06634849550938926</v>
+        <v>0.01650168187916279</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01266819304790091</v>
+        <v>0.001044479420497373</v>
       </c>
     </row>
     <row r="4">
@@ -620,35 +620,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(0.0848, 0.124]</t>
+          <t>(0.0239, 0.0431]</t>
         </is>
       </c>
       <c r="C4" t="n">
         <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>10.6</v>
+        <v>8.799999999999999</v>
       </c>
       <c r="E4" t="n">
         <v>400</v>
       </c>
       <c r="F4" t="n">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5999999999999992</v>
+        <v>-1.200000000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0003496134487438532</v>
+        <v>0.001534000458118622</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1039648413139609</v>
+        <v>0.03172575309872627</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1058387792695563</v>
+        <v>0.03246678039431572</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01301780649664477</v>
+        <v>0.002578479878615994</v>
       </c>
     </row>
     <row r="5">
@@ -657,35 +657,35 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(0.124, 0.176]</t>
+          <t>(0.0431, 0.0698]</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>10.05</v>
       </c>
       <c r="D5" t="n">
-        <v>11.6</v>
+        <v>11.2</v>
       </c>
       <c r="E5" t="n">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="F5" t="n">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G5" t="n">
-        <v>1.6</v>
+        <v>1.15</v>
       </c>
       <c r="H5" t="n">
-        <v>0.002374720081892372</v>
+        <v>0.001245923153653587</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1503823417554057</v>
+        <v>0.05581361427903175</v>
       </c>
       <c r="J5" t="n">
-        <v>0.1498032409048426</v>
+        <v>0.05511580035090446</v>
       </c>
       <c r="K5" t="n">
-        <v>0.01539252657853714</v>
+        <v>0.003824403032269581</v>
       </c>
     </row>
     <row r="6">
@@ -694,35 +694,35 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(0.176, 0.232]</t>
+          <t>(0.0698, 0.121]</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10.15</v>
+        <v>9.950000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>10.5</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E6" t="n">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="F6" t="n">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3499999999999989</v>
+        <v>-0.1500000000000001</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0001186554308648838</v>
+        <v>2.278524824096287e-05</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2071092720163349</v>
+        <v>0.09360076487064362</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2083824026639225</v>
+        <v>0.09032906591892242</v>
       </c>
       <c r="K6" t="n">
-        <v>0.01551118200940202</v>
+        <v>0.003847188280510544</v>
       </c>
     </row>
     <row r="7">
@@ -731,35 +731,35 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(0.232, 0.297]</t>
+          <t>(0.121, 0.196]</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10.625</v>
+        <v>10.15</v>
       </c>
       <c r="D7" t="n">
-        <v>10.1</v>
+        <v>10.3</v>
       </c>
       <c r="E7" t="n">
-        <v>425</v>
+        <v>406</v>
       </c>
       <c r="F7" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.524999999999999</v>
+        <v>0.1499999999999987</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0002660400275571495</v>
+        <v>2.200528462169025e-05</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2677401298997946</v>
+        <v>0.1576640456914902</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2667596301300774</v>
+        <v>0.1617581695318222</v>
       </c>
       <c r="K7" t="n">
-        <v>0.01577722203695917</v>
+        <v>0.003869193565132234</v>
       </c>
     </row>
     <row r="8">
@@ -768,35 +768,35 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(0.297, 0.34]</t>
+          <t>(0.196, 0.306]</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9.225</v>
+        <v>9.875</v>
       </c>
       <c r="D8" t="n">
-        <v>6.9</v>
+        <v>9.4</v>
       </c>
       <c r="E8" t="n">
-        <v>369</v>
+        <v>395</v>
       </c>
       <c r="F8" t="n">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="G8" t="n">
-        <v>-2.324999999999999</v>
+        <v>-0.4750000000000004</v>
       </c>
       <c r="H8" t="n">
-        <v>0.006751701846018515</v>
+        <v>0.0002341589521783303</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3226663771875953</v>
+        <v>0.2552129626274109</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3237137989686228</v>
+        <v>0.253635436296463</v>
       </c>
       <c r="K8" t="n">
-        <v>0.02252892388297769</v>
+        <v>0.004103352517310564</v>
       </c>
     </row>
     <row r="9">
@@ -805,35 +805,35 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(0.34, 0.415]</t>
+          <t>(0.306, 0.44]</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>10.15</v>
       </c>
       <c r="D9" t="n">
-        <v>11.1</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="F9" t="n">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="G9" t="n">
-        <v>1.1</v>
+        <v>-2.15</v>
       </c>
       <c r="H9" t="n">
-        <v>0.001147960168566669</v>
+        <v>0.005117691521871152</v>
       </c>
       <c r="I9" t="n">
-        <v>0.3813352370607807</v>
+        <v>0.3768987655639648</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3779666229987125</v>
+        <v>0.3747358918190002</v>
       </c>
       <c r="K9" t="n">
-        <v>0.02367688405154435</v>
+        <v>0.009221044039181716</v>
       </c>
     </row>
     <row r="10">
@@ -842,35 +842,35 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(0.415, 0.504]</t>
+          <t>(0.44, 0.686]</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>9.825000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E10" t="n">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="F10" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.000000000000001</v>
+        <v>1.175</v>
       </c>
       <c r="H10" t="n">
-        <v>0.001053605156578265</v>
+        <v>0.001327340101755786</v>
       </c>
       <c r="I10" t="n">
-        <v>0.4533420113984608</v>
+        <v>0.5581108331680298</v>
       </c>
       <c r="J10" t="n">
-        <v>0.4515532226007673</v>
+        <v>0.5460732579231262</v>
       </c>
       <c r="K10" t="n">
-        <v>0.02473048920812262</v>
+        <v>0.0105483841409375</v>
       </c>
     </row>
     <row r="11">
@@ -879,35 +879,35 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>(0.504, 1.0]</t>
+          <t>(0.686, 1.0]</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>11.3</v>
+        <v>10.8</v>
       </c>
       <c r="E11" t="n">
         <v>400</v>
       </c>
       <c r="F11" t="n">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G11" t="n">
-        <v>1.3</v>
+        <v>0.7999999999999994</v>
       </c>
       <c r="H11" t="n">
-        <v>0.001588829225415238</v>
+        <v>0.000615688329089025</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5941048113759376</v>
+        <v>0.822874903678894</v>
       </c>
       <c r="J11" t="n">
-        <v>0.5929630301681337</v>
+        <v>0.8338835835456848</v>
       </c>
       <c r="K11" t="n">
-        <v>0.02631931843353786</v>
+        <v>0.01116407247002653</v>
       </c>
     </row>
   </sheetData>
@@ -944,21 +944,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>feature_46</t>
+          <t>feature_26</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1801049023590067</v>
+        <v>0.1719878911972046</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>feature_26</t>
+          <t>feature_46</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.179777020607258</v>
+        <v>0.1675053536891937</v>
       </c>
     </row>
     <row r="4">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1596645977419233</v>
+        <v>0.1633881777524948</v>
       </c>
     </row>
     <row r="5">
@@ -978,7 +978,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.145942860528923</v>
+        <v>0.1343928128480911</v>
       </c>
     </row>
     <row r="6">
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1204538596149496</v>
+        <v>0.1252419352531433</v>
       </c>
     </row>
     <row r="7">
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1151390752416003</v>
+        <v>0.1250054389238358</v>
       </c>
     </row>
     <row r="8">
@@ -1008,7 +1008,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.09891768390633918</v>
+        <v>0.1124783754348755</v>
       </c>
     </row>
   </sheetData>
@@ -1607,45 +1607,45 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>[-12.02, -5.19]</t>
+          <t>[-12.02, -5.16]</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.4772809145481526</v>
+        <v>-0.5098482432106972</v>
       </c>
       <c r="C2" t="n">
         <v>27</v>
       </c>
       <c r="D2" t="n">
-        <v>362</v>
+        <v>374</v>
       </c>
       <c r="E2" t="n">
-        <v>0.06940874035989718</v>
+        <v>0.06733167082294264</v>
       </c>
       <c r="F2" t="n">
-        <v>0.01841403241313921</v>
+        <v>0.02138621439839053</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>[-5.19, -3.88]</t>
+          <t>[-5.16, -3.88]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.953790428154294</v>
+        <v>-0.9829702172630708</v>
       </c>
       <c r="C3" t="n">
         <v>17</v>
       </c>
       <c r="D3" t="n">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04381443298969072</v>
+        <v>0.04260651629072681</v>
       </c>
       <c r="F3" t="n">
-        <v>0.06108144140435337</v>
+        <v>0.06598229373534219</v>
       </c>
     </row>
     <row r="4">
@@ -1655,85 +1655,85 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.3275902612284237</v>
+        <v>-0.2614816422153408</v>
       </c>
       <c r="C4" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" t="n">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="E4" t="n">
-        <v>0.07989690721649484</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>0.009174059519922353</v>
+        <v>0.006183460215060842</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>[-2.93, -2.10]</t>
+          <t>[-2.93, -2.12]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.6010356065651006</v>
+        <v>-0.6306873746152155</v>
       </c>
       <c r="C5" t="n">
         <v>24</v>
       </c>
       <c r="D5" t="n">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06169665809768637</v>
+        <v>0.06</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02782983166207104</v>
+        <v>0.03114827565808744</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[-2.10, -1.26]</t>
+          <t>[-2.12, -1.27]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.2879107015624391</v>
+        <v>-0.3606056394826176</v>
       </c>
       <c r="C6" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" t="n">
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="E6" t="n">
-        <v>0.08290155440414508</v>
+        <v>0.0775</v>
       </c>
       <c r="F6" t="n">
-        <v>0.007160287460904231</v>
+        <v>0.01131212396800935</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[-1.26, -0.53]</t>
+          <t>[-1.27, -0.53]</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.1419849972862109</v>
+        <v>-0.1096337297438762</v>
       </c>
       <c r="C7" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" t="n">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="E7" t="n">
-        <v>0.09487179487179487</v>
+        <v>0.09774436090225563</v>
       </c>
       <c r="F7" t="n">
-        <v>0.001863056755208459</v>
+        <v>0.001150861669558705</v>
       </c>
     </row>
     <row r="8">
@@ -1743,19 +1743,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0800827693685522</v>
+        <v>0.0674846184240665</v>
       </c>
       <c r="C8" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D8" t="n">
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="E8" t="n">
-        <v>0.115979381443299</v>
+        <v>0.114713216957606</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0006431753134246425</v>
+        <v>0.0004696824854299417</v>
       </c>
     </row>
     <row r="9">
@@ -1765,63 +1765,63 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.2215738524311573</v>
+        <v>0.2304745439711655</v>
       </c>
       <c r="C9" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9" t="n">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1314432989690722</v>
+        <v>0.1325</v>
       </c>
       <c r="F9" t="n">
-        <v>0.005201536452765423</v>
+        <v>0.005821395375469932</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>[1.17, 2.63]</t>
+          <t>[1.17, 2.65]</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2871213771749666</v>
+        <v>0.2729479326187155</v>
       </c>
       <c r="C10" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" t="n">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1391752577319588</v>
+        <v>0.1375</v>
       </c>
       <c r="F10" t="n">
-        <v>0.008957446217250429</v>
+        <v>0.008299339271090993</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[2.63, 12.45]</t>
+          <t>[2.65, 12.45]</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.096502597382852</v>
+        <v>1.12244209854006</v>
       </c>
       <c r="C11" t="n">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D11" t="n">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2673521850899743</v>
+        <v>0.2725</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1750206802072485</v>
+        <v>0.1901445399464467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>